<commit_message>
update FeatherWing Implementation Chart
</commit_message>
<xml_diff>
--- a/docs/FeatherWing_Implementation_Chart.xlsx
+++ b/docs/FeatherWing_Implementation_Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\Documents\GitHub\AD9833_FeatherWing_ADSR\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\Documents\GitHub\AD9833_ADSR_FeatherWing\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1933AEDA-5864-49E5-B542-2E62F1D13D38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7EDC2F-290B-4F32-9C66-262E4FBED99E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="-14910" windowWidth="21645" windowHeight="14340" xr2:uid="{C7EDD24A-D5F0-40E7-9C67-C76A930CACB0}"/>
+    <workbookView xWindow="5175" yWindow="720" windowWidth="21960" windowHeight="14865" xr2:uid="{C7EDD24A-D5F0-40E7-9C67-C76A930CACB0}"/>
   </bookViews>
   <sheets>
     <sheet name="FeatherWing Impl Chart" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>FeatherWing Implementation Chart</t>
   </si>
@@ -191,7 +191,7 @@
     <t>SCL</t>
   </si>
   <si>
-    <t>X</t>
+    <t>I/O</t>
   </si>
 </sst>
 </file>
@@ -820,7 +820,7 @@
   <dimension ref="B2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>